<commit_message>
Added story points to user stories spreadsheet
</commit_message>
<xml_diff>
--- a/Project Planning/User stories final.xlsx
+++ b/Project Planning/User stories final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3da2344c20c04f1c/Desktop/QUT/2025-1/CAB302/Main project resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3da2344c20c04f1c/Desktop/QUT/2025-1/CAB302/CAB302 main project new/CAB203_A1_Project_New/Project Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{AEECFC1A-B7BE-42BD-9E0F-CE0970812D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9108A35E-F459-4BCB-9696-C76A4FAB5055}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{AEECFC1A-B7BE-42BD-9E0F-CE0970812D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF88C3EB-4508-4B98-B4D6-E42F7800712F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{EB63D5DF-D502-4E24-9D29-12BD7DAA2616}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>User story</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>As a user, I want to be able to assign each quiz to the topic/subject it belongs to so that I can easily find what I am looking for.</t>
+  </si>
+  <si>
+    <t>Story points</t>
   </si>
 </sst>
 </file>
@@ -278,14 +281,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -294,30 +296,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -422,193 +401,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA45200"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA45200"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA45200"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -659,11 +451,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0824BF8F-8EC8-488E-856B-A003B8554D7E}" name="Table1" displayName="Table1" ref="A1:B32" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A1:B32" xr:uid="{0824BF8F-8EC8-488E-856B-A003B8554D7E}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0824BF8F-8EC8-488E-856B-A003B8554D7E}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:C32" xr:uid="{0824BF8F-8EC8-488E-856B-A003B8554D7E}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B7D81835-8B91-4B85-A41C-C47BCC7B0B5D}" name="User story"/>
     <tableColumn id="2" xr3:uid="{10EC962A-A2CE-4CA3-8B6C-34AEC721A622}" name="Priority"/>
+    <tableColumn id="3" xr3:uid="{BE203CA2-DBC4-4E23-90AC-625A75AEC0F0}" name="Story points"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -989,54 +782,70 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="157.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="157.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.59765625" customWidth="1"/>
     <col min="6" max="6" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
@@ -1044,239 +853,317 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>4</v>
       </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
+      <c r="C18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+      <c r="C21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B32" xr:uid="{ADABA6AD-1965-4F13-8D28-073500A1E241}">
-      <formula1>$F$6:$F$9</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{69EFEC2B-FFAA-470A-A6AD-B81F367C146D}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B32" xr:uid="{ADABA6AD-1965-4F13-8D28-073500A1E241}">
       <formula1>$F$6:$F$9</formula1>
     </dataValidation>
   </dataValidations>
@@ -1288,6 +1175,36 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{245C099C-E5F1-4B86-A006-2CD31EB6824A}">
+            <xm:f>NOT(ISERROR(SEARCH($F$9,B2)))</xm:f>
+            <xm:f>$F$9</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="thin">
+                  <color auto="1"/>
+                </left>
+                <right style="thin">
+                  <color auto="1"/>
+                </right>
+                <top style="thin">
+                  <color auto="1"/>
+                </top>
+                <bottom style="thin">
+                  <color auto="1"/>
+                </bottom>
+                <vertical/>
+                <horizontal/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="containsText" priority="2" operator="containsText" id="{AA8A5FEC-9EE8-4501-8A6E-D8FC63DC82B3}">
             <xm:f>NOT(ISERROR(SEARCH($F$8,B2)))</xm:f>
             <xm:f>$F$8</xm:f>
@@ -1376,36 +1293,6 @@
               </border>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{245C099C-E5F1-4B86-A006-2CD31EB6824A}">
-            <xm:f>NOT(ISERROR(SEARCH($F$9,B2)))</xm:f>
-            <xm:f>$F$9</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-              <border>
-                <left style="thin">
-                  <color auto="1"/>
-                </left>
-                <right style="thin">
-                  <color auto="1"/>
-                </right>
-                <top style="thin">
-                  <color auto="1"/>
-                </top>
-                <bottom style="thin">
-                  <color auto="1"/>
-                </bottom>
-                <vertical/>
-                <horizontal/>
-              </border>
-            </x14:dxf>
-          </x14:cfRule>
           <xm:sqref>B2:B32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>

</xml_diff>